<commit_message>
Entrega Final - Reto 4
</commit_message>
<xml_diff>
--- a/Docs/Documento de Análisis - Reto 4.xlsx
+++ b/Docs/Documento de Análisis - Reto 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee7300ab24533284/Documentos/Extras/MEL - EDA/Repositorios Dañados/Reto4-G19/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{6E8D1ECB-07A5-4D6B-94C5-34CE038B89BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E658011-F3D8-4566-BDFA-7922BAC1ECBF}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{6E8D1ECB-07A5-4D6B-94C5-34CE038B89BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3A9AD8F-E2BF-480A-9A5C-F404A1678847}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{6CA6B4F5-C0DE-5F41-8226-6FA006D8C271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{6CA6B4F5-C0DE-5F41-8226-6FA006D8C271}"/>
   </bookViews>
   <sheets>
     <sheet name="Requerimiento1" sheetId="1" r:id="rId1"/>
@@ -1884,8 +1884,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.0085533623929977E-3"/>
-                  <c:y val="-6.2834884404031469E-2"/>
+                  <c:x val="4.1339854635257037E-2"/>
+                  <c:y val="9.0276336369965543E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1956,6 +1956,30 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>436.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1638.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2564.1999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10176.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15865.1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7388,8 +7412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2714FA2B-2EDE-024D-B1B5-1B1F0A1A3EDE}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7426,7 +7450,9 @@
       <c r="C2" s="1">
         <v>181</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3">
+        <v>62.5</v>
+      </c>
       <c r="E2" s="1">
         <v>2937.5</v>
       </c>
@@ -7441,7 +7467,9 @@
       <c r="C3" s="1">
         <v>453</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3">
+        <v>103.7</v>
+      </c>
       <c r="E3" s="1">
         <v>2953.12</v>
       </c>
@@ -7456,7 +7484,9 @@
       <c r="C4" s="1">
         <v>907</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3">
+        <v>250</v>
+      </c>
       <c r="E4" s="1">
         <v>3343.75</v>
       </c>
@@ -7471,7 +7501,9 @@
       <c r="C5" s="1">
         <v>1815</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3">
+        <v>436.8</v>
+      </c>
       <c r="E5" s="1">
         <v>3687.5</v>
       </c>
@@ -7486,7 +7518,9 @@
       <c r="C6" s="1">
         <v>2722</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3">
+        <v>1638.7</v>
+      </c>
       <c r="E6" s="1">
         <v>4796.88</v>
       </c>
@@ -7501,7 +7535,9 @@
       <c r="C7" s="1">
         <v>4537</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3">
+        <v>2564.1999999999998</v>
+      </c>
       <c r="E7" s="1">
         <v>9734.3799999999992</v>
       </c>
@@ -7516,7 +7552,9 @@
       <c r="C8" s="1">
         <v>7260</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>10176.799999999999</v>
+      </c>
       <c r="E8" s="1">
         <v>21250</v>
       </c>
@@ -7531,7 +7569,9 @@
       <c r="C9" s="1">
         <v>9075</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3">
+        <v>15865.1</v>
+      </c>
       <c r="E9" s="1">
         <v>40578.120000000003</v>
       </c>
@@ -7546,8 +7586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BA4576-C5C0-204C-94E8-3E6936BE302C}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="A1:E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>